<commit_message>
Method names and graph queries
The search method names have changed to findXXXByPropertyValue and the graph-like queries are now optional
</commit_message>
<xml_diff>
--- a/compliance/repository-compliance/Open Metadata - Repository Compliance Workbook.xlsx
+++ b/compliance/repository-compliance/Open Metadata - Repository Compliance Workbook.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1640" yWindow="2620" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
+    <workbookView xWindow="2880" yWindow="0" windowWidth="25600" windowHeight="16840" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Compliance Requirements" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="81">
   <si>
     <t>Functional Matrix</t>
   </si>
@@ -98,34 +98,6 @@
 undoRelationshipUpdate()</t>
   </si>
   <si>
-    <t xml:space="preserve">isEntityKnown()
-getEntitySummary()
-getEntityDetail()
-getRelationshipsForEntity()
-findEntitiesByProperty()
-findEntitiesByClassification()
-searchForEntities()
-isRelationshipKnown()
-getRelationship()
-findRelationshipsByProperty()
-searchForRelationships()
-getLinkingEntities()
-getEntityNeighborhood()
-getRelatedEntities()
-addEntity()
-updateEntityStatus()
-updateEntityProperties()
-purgeEntity()
-classifyEntity()
-declassifyEntity()
-updateEntityClassification()
-addRelationship()
-updateRelationshipStatus()
-updateRelationshipProperties()
-purgeRelationship()
-</t>
-  </si>
-  <si>
     <t>deleteEntity()
 restoreEntity()
 deleteRelationship()
@@ -145,20 +117,6 @@
   </si>
   <si>
     <t>Historical queries</t>
-  </si>
-  <si>
-    <t>asOfTime parameter on following calls:
- * getEntityDetail()
- * getRelationshipsForEntity()
- * findEntitiesByProperty()
- * findEntitiesByClassification()
- * searchForEntities()
- * getRelationship()
- * findRelationshipsByProperty()
- * searchForRelationships()
- * getLinkingEntities()
- * getEntityNeighborhood()
- * getRelatedEntities()</t>
   </si>
   <si>
     <t>Throw FunctionNotSupportedException on method where asOfTime parameter is not null.</t>
@@ -230,6 +188,87 @@
   </si>
   <si>
     <t>The OMRS includes functions that can provide support for all of these methods.  A specific metadata reposiotry needs to add the necessary configuration and support to ensure it can store, locate and maintain instances of the types it declares it can support.</t>
+  </si>
+  <si>
+    <t>Dynamic type definitions enable open metadata solutions to dynamically extend the function of a metadata server.  The type definitions are maintained in an open metadata archive and loaded into the repository on server start up or administative command.  Once loaded , the repository connector should treat these types as if they were native types.</t>
+  </si>
+  <si>
+    <t>Historical queries enables a user to review the state that their data and systems were in in the past.  It requires the repository to maintain details of each version of its metadata instances and enable queries on them.</t>
+  </si>
+  <si>
+    <t>Versioning</t>
+  </si>
+  <si>
+    <t>Ability to increment a version number within each metadata element, each time it is changed.</t>
+  </si>
+  <si>
+    <t>All create, update, delete, undo, restore method should increment the version number.</t>
+  </si>
+  <si>
+    <t>Type enforcement</t>
+  </si>
+  <si>
+    <t>Ability to ensure metadata instance conform to their type definition.</t>
+  </si>
+  <si>
+    <t>All create and update requests should validate that new properties, statuses, relationships and classifications conform to the definition in their corresponding types.</t>
+  </si>
+  <si>
+    <t>Re-homing involves updating the metadata collection Id in the metadata instance.  This affects which metadata reposiotry can edit the metadata instance.</t>
+  </si>
+  <si>
+    <t>Re-typing is useful to remove instances from types that need to be updated or deleted.  The instance must still be valid for its new type.</t>
+  </si>
+  <si>
+    <t>Re-identification is used to resolve conflicts where two different repositories assign the sam unique identifier to two different instances.  It is good to have at least on repository in a cohort that supports re-identification, or such conflicts require one of the instances to be deleted and recreated to resolve the conflicts.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Undo restores the previous version of an instance to its previous state (except that the version number is incremented).  </t>
+  </si>
+  <si>
+    <t>Entity proxies enable relationships to be stored in a repository even when the entity is not stored locally.</t>
+  </si>
+  <si>
+    <t>Soft-delete enables metadata that is officially deleted to remain to support historical queries and undos of deletes.</t>
+  </si>
+  <si>
+    <t>Examples</t>
+  </si>
+  <si>
+    <t>Enterprise OMRS Connector</t>
+  </si>
+  <si>
+    <t>Not Supported</t>
+  </si>
+  <si>
+    <t>Local OMRS Connector</t>
+  </si>
+  <si>
+    <t>Supported (delegated to underlying repository connectors).</t>
+  </si>
+  <si>
+    <t>Supported</t>
+  </si>
+  <si>
+    <t>In-memory Repository Connector</t>
+  </si>
+  <si>
+    <t>Atlas</t>
+  </si>
+  <si>
+    <t>Not supported (work in progress)</t>
+  </si>
+  <si>
+    <t>Not supported ?</t>
+  </si>
+  <si>
+    <t>IGC</t>
+  </si>
+  <si>
+    <t>Not supported</t>
+  </si>
+  <si>
+    <t>REST Connector</t>
   </si>
   <si>
     <r>
@@ -245,114 +284,77 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Note to reviewers</t>
+      <t/>
     </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> - should support for classifications and/or relationships be optional?</t>
-    </r>
-  </si>
-  <si>
-    <t>Dynamic type definitions enable open metadata solutions to dynamically extend the function of a metadata server.  The type definitions are maintained in an open metadata archive and loaded into the repository on server start up or administative command.  Once loaded , the repository connector should treat these types as if they were native types.</t>
-  </si>
-  <si>
-    <t>Historical queries enables a user to review the state that their data and systems were in in the past.  It requires the repository to maintain details of each version of its metadata instances and enable queries on them.</t>
-  </si>
-  <si>
-    <t>Versioning</t>
-  </si>
-  <si>
-    <t>Ability to increment a version number within each metadata element, each time it is changed.</t>
-  </si>
-  <si>
-    <t>All create, update, delete, undo, restore method should increment the version number.</t>
-  </si>
-  <si>
-    <t>Type enforcement</t>
-  </si>
-  <si>
-    <t>Ability to ensure metadata instance conform to their type definition.</t>
-  </si>
-  <si>
-    <t>All create and update requests should validate that new properties, statuses, relationships and classifications conform to the definition in their corresponding types.</t>
-  </si>
-  <si>
-    <t>Reference copies should include the metadata collectin id of their home repository and should be read only.</t>
-  </si>
-  <si>
-    <t>Re-homing involves updating the metadata collection Id in the metadata instance.  This affects which metadata reposiotry can edit the metadata instance.</t>
-  </si>
-  <si>
-    <t>Re-typing is useful to remove instances from types that need to be updated or deleted.  The instance must still be valid for its new type.</t>
-  </si>
-  <si>
-    <t>Re-identification is used to resolve conflicts where two different repositories assign the sam unique identifier to two different instances.  It is good to have at least on repository in a cohort that supports re-identification, or such conflicts require one of the instances to be deleted and recreated to resolve the conflicts.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Undo restores the previous version of an instance to its previous state (except that the version number is incremented).  </t>
-  </si>
-  <si>
-    <t>Entity proxies enable relationships to be stored in a repository even when the entity is not stored locally.</t>
-  </si>
-  <si>
-    <t>Soft-delete enables metadata that is officially deleted to remain to support historical queries and undos of deletes.</t>
-  </si>
-  <si>
-    <t>Examples</t>
-  </si>
-  <si>
-    <t>Enterprise OMRS Connector</t>
-  </si>
-  <si>
-    <t>Not Supported</t>
-  </si>
-  <si>
-    <t>Local OMRS Connector</t>
-  </si>
-  <si>
-    <t>Supported (delegated to underlying repository connectors).</t>
-  </si>
-  <si>
-    <t>Supported</t>
-  </si>
-  <si>
-    <t>In-memory Repository Connector</t>
-  </si>
-  <si>
-    <t>Atlas</t>
-  </si>
-  <si>
-    <t>Not supported (work in progress)</t>
-  </si>
-  <si>
-    <t>Not supported ?</t>
-  </si>
-  <si>
-    <t>IGC</t>
-  </si>
-  <si>
-    <t>Not supported</t>
-  </si>
-  <si>
-    <t>REST Connector</t>
+  </si>
+  <si>
+    <t>Reference copies should include the metadata collection id of their home repository and should be read only.</t>
+  </si>
+  <si>
+    <t>getLinkingEntities()
+getEntityNeighborhood()
+getRelatedEntities()</t>
+  </si>
+  <si>
+    <t>Graph-type queries</t>
+  </si>
+  <si>
+    <t>Ability to understand the relationships throughout the metadata using graph-like queries.</t>
+  </si>
+  <si>
+    <t>Graph-type queries traverse multiple relationships in the metadata.  For some repositories this may result in a high load from these types of queries.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">isEntityKnown()
+getEntitySummary()
+getEntityDetail()
+getRelationshipsForEntity()
+findEntitiesByProperty()
+findEntitiesByClassification()
+findEntitiesByPropertyValue()
+isRelationshipKnown()
+getRelationship()
+findRelationshipsByProperty()
+findRelationshipsByPropertyValue()
+addEntity()
+updateEntityStatus()
+updateEntityProperties()
+purgeEntity()
+classifyEntity()
+declassifyEntity()
+updateEntityClassification()
+addRelationship()
+updateRelationshipStatus()
+updateRelationshipProperties()
+purgeRelationship()
+</t>
+  </si>
+  <si>
+    <t>asOfTime parameter on following calls:
+ * getEntityDetail()
+ * getRelationshipsForEntity()
+ * findEntitiesByProperty()
+ * findEntitiesByClassification()
+ * findEntitiesByPropertyValue()
+ * getRelationship()
+ * findRelationshipsByProperty()
+ * findRelationshipsByPropetyValue()
+ * getLinkingEntities()
+ * getEntityNeighborhood()
+ * getRelatedEntities()</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -383,6 +385,24 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -422,11 +442,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -456,9 +478,11 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="6">
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
+    <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -791,8 +815,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:K30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="24.33203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -841,7 +865,7 @@
         <v>12</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="387" customHeight="1">
@@ -852,391 +876,425 @@
         <v>16</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>19</v>
+        <v>79</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>48</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="70" customHeight="1">
       <c r="A10" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="92" customHeight="1">
       <c r="A11" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="16" customHeight="1"/>
-    <row r="13" spans="1:11" s="3" customFormat="1" ht="16" customHeight="1">
-      <c r="A13" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" s="3" customFormat="1" ht="16" customHeight="1">
+      <c r="A12" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F13" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" s="2" customFormat="1" ht="33" customHeight="1">
-      <c r="A14" s="2" t="s">
+      <c r="F12" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" s="2" customFormat="1" ht="33" customHeight="1">
+      <c r="A13" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B13" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C13" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D13" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E13" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="F13" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="150">
+      <c r="A14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="I14" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="G14" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="H14" s="2" t="s">
+      <c r="J14" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="62" customHeight="1">
+      <c r="A15" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="I14" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="J14" s="2" t="s">
+      <c r="B15" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="K15" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="K14" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="150">
-      <c r="A15" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="K15" s="1" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="206" customHeight="1">
       <c r="A16" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="E16" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F16" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="J16" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="G16" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>72</v>
-      </c>
       <c r="K16" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="60">
       <c r="A17" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="I17" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="J17" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="J17" s="1" t="s">
-        <v>73</v>
-      </c>
       <c r="K17" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="60">
       <c r="A18" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="60">
       <c r="A19" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>37</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="I19" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="J19" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="J19" s="1" t="s">
-        <v>73</v>
-      </c>
       <c r="K19" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="135">
       <c r="A20" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="C20" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="I20" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="J20" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="J20" s="1" t="s">
-        <v>73</v>
-      </c>
       <c r="K20" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="60">
       <c r="A21" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="I21" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="J21" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="J21" s="1" t="s">
-        <v>73</v>
-      </c>
       <c r="K21" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="75">
       <c r="A22" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="I22" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="J22" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="J22" s="1" t="s">
-        <v>73</v>
-      </c>
       <c r="K22" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="90">
       <c r="A23" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>57</v>
+        <v>74</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="G23" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="J23" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="H23" s="1" t="s">
+      <c r="K23" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="J23" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="K23" s="1" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="26" spans="1:11" s="6" customFormat="1" ht="20" thickBot="1">
@@ -1258,7 +1316,7 @@
         <v>2</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="30" spans="1:11">
@@ -1266,11 +1324,12 @@
         <v>3</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>